<commit_message>
Fixed Reload Menu Button to reload current scene
</commit_message>
<xml_diff>
--- a/Assets/Excercises/Default/TruthTables.xlsx
+++ b/Assets/Excercises/Default/TruthTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weberrh\Desktop\BA\BA22\BA22-knaa-03\Assets\Excercises\Default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73D4A1F8-F086-48F0-9B88-FC60771F09D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B78D74-9E3F-4323-969D-E0545AEFFDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{043328BC-87EE-46A7-935B-7C4E799ED94B}"/>
+    <workbookView xWindow="25490" yWindow="3490" windowWidth="19420" windowHeight="10420" xr2:uid="{043328BC-87EE-46A7-935B-7C4E799ED94B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>A</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>O1</t>
+  </si>
+  <si>
+    <t>HALFADDER</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>FULLADDER</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -103,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -126,12 +138,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -140,12 +178,350 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="26"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="26"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -735,78 +1111,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{49FF496C-E8A0-4B1D-8D49-BC475C4C814D}" name="Table1" displayName="Table1" ref="A3:C7" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{49FF496C-E8A0-4B1D-8D49-BC475C4C814D}" name="Table1" displayName="Table1" ref="A3:C7" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A3:C7" xr:uid="{49FF496C-E8A0-4B1D-8D49-BC475C4C814D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{100ADB5E-B999-47B2-B055-B725D60CB010}" name="A" totalsRowLabel="Total" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E0FABA55-6A84-4AC4-A41D-32A0336A0BA4}" name="B" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{BAAF3FC6-B87E-4FBE-BBA3-84DC8ED52CAA}" name="O1" totalsRowFunction="count" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{100ADB5E-B999-47B2-B055-B725D60CB010}" name="A" totalsRowLabel="Total" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{E0FABA55-6A84-4AC4-A41D-32A0336A0BA4}" name="B" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{BAAF3FC6-B87E-4FBE-BBA3-84DC8ED52CAA}" name="O1" totalsRowFunction="count" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2446AE41-65D3-4C3E-8537-063C33C8B463}" name="Table13" displayName="Table13" ref="A12:C16" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2446AE41-65D3-4C3E-8537-063C33C8B463}" name="Table13" displayName="Table13" ref="A12:C16" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A12:C16" xr:uid="{2446AE41-65D3-4C3E-8537-063C33C8B463}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{898A971F-43CD-40ED-8DDD-46F6274F299E}" name="A" totalsRowLabel="Total" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{A1CCC852-6ED6-47BA-8205-5E2E6F938CCE}" name="B" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{B95B8EBF-8615-4A43-A2ED-2AEEFA10C7B0}" name="O1" totalsRowFunction="count" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{898A971F-43CD-40ED-8DDD-46F6274F299E}" name="A" totalsRowLabel="Total" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{A1CCC852-6ED6-47BA-8205-5E2E6F938CCE}" name="B" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{B95B8EBF-8615-4A43-A2ED-2AEEFA10C7B0}" name="O1" totalsRowFunction="count" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AB9E469-9A81-47E4-BF10-EC65C2308D12}" name="Table134" displayName="Table134" ref="A21:C25" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AB9E469-9A81-47E4-BF10-EC65C2308D12}" name="Table134" displayName="Table134" ref="A21:C25" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A21:C25" xr:uid="{0AB9E469-9A81-47E4-BF10-EC65C2308D12}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{05B40532-C26C-4523-ADCD-465B3B89CA04}" name="A" totalsRowLabel="Total" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C1EEEFC9-928F-4869-BE8A-C1F5B30023F5}" name="B" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{4835E406-539D-4AAF-8A9A-8D71E2C196A7}" name="O1" totalsRowFunction="count" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{05B40532-C26C-4523-ADCD-465B3B89CA04}" name="A" totalsRowLabel="Total" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{C1EEEFC9-928F-4869-BE8A-C1F5B30023F5}" name="B" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{4835E406-539D-4AAF-8A9A-8D71E2C196A7}" name="O1" totalsRowFunction="count" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C37617F6-D0E2-4E3B-9DAD-9763E342B800}" name="Table1345" displayName="Table1345" ref="A30:C34" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C37617F6-D0E2-4E3B-9DAD-9763E342B800}" name="Table1345" displayName="Table1345" ref="A30:C34" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A30:C34" xr:uid="{C37617F6-D0E2-4E3B-9DAD-9763E342B800}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D33D8966-3FE1-4A8C-9C67-6BE4522212BF}" name="A" totalsRowLabel="Total" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{78417A46-EACC-4D65-8B54-F395834B1EF5}" name="B" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{6FE36B92-A2C2-4F16-85E4-E39C91AD3FD9}" name="O1" totalsRowFunction="count" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{D33D8966-3FE1-4A8C-9C67-6BE4522212BF}" name="A" totalsRowLabel="Total" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{78417A46-EACC-4D65-8B54-F395834B1EF5}" name="B" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{6FE36B92-A2C2-4F16-85E4-E39C91AD3FD9}" name="O1" totalsRowFunction="count" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D87BE111-8FC6-4283-8ABC-165BFFD90E49}" name="Table13456" displayName="Table13456" ref="A39:B41" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D87BE111-8FC6-4283-8ABC-165BFFD90E49}" name="Table13456" displayName="Table13456" ref="A39:B41" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A39:B41" xr:uid="{D87BE111-8FC6-4283-8ABC-165BFFD90E49}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3F711ED9-D41D-4403-B3A4-F161C517DEC1}" name="A" totalsRowLabel="Total" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{0FC0BD61-0FD7-41C0-8213-E3F58587EEFC}" name="O1" totalsRowFunction="count" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3F711ED9-D41D-4403-B3A4-F161C517DEC1}" name="A" totalsRowLabel="Total" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{0FC0BD61-0FD7-41C0-8213-E3F58587EEFC}" name="O1" totalsRowFunction="count" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D87B2B44-56F5-41F2-A2D7-4148B442B7BE}" name="Table13457" displayName="Table13457" ref="A47:D51" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A47:D51" xr:uid="{D87B2B44-56F5-41F2-A2D7-4148B442B7BE}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5DB0CC7A-E839-486A-B956-4431694A1B3E}" name="A" totalsRowLabel="Total" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B3C0478E-9963-42CB-B80B-0E56F187170A}" name="B" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{D7CE7ABA-9996-4C61-8084-3CC2267802EB}" name="O1" totalsRowFunction="count" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{5A164BBD-FF08-4AE2-A0F4-BEA87FD156AF}" name="O2" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{055CCDE3-CC02-4420-91C7-EBEF8CDC066F}" name="Table134578" displayName="Table134578" ref="A57:E65" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A57:E65" xr:uid="{055CCDE3-CC02-4420-91C7-EBEF8CDC066F}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{DC53C094-5492-47D2-BC0A-5E7C05A3CB54}" name="A" totalsRowLabel="Total" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{4FAFE96B-58BA-4EDB-A4D9-F1318FF431F8}" name="B" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C78BC8E0-4C49-4B46-A00A-C00A9296FE9D}" name="C" totalsRowFunction="count" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{2C436095-982D-45EB-8D43-6CFE99CEF2EF}" name="O1" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{678B99BF-6466-45BE-88C2-4799305236CE}" name="O2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1109,15 +1523,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D958E6-50B5-4E72-8798-411F7678279F}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="12.7109375" customWidth="1"/>
+    <col min="1" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
@@ -1338,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -1349,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -1360,12 +1774,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A40" s="2">
         <v>0</v>
       </c>
@@ -1381,23 +1795,258 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A41" s="2">
         <v>1</v>
       </c>
       <c r="B41" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A48" s="2">
+        <v>0</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A49" s="2">
+        <v>0</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A50" s="2">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A51" s="2">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A57" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A58" s="2">
+        <v>0</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
+      </c>
+      <c r="E58" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A59" s="2">
+        <v>0</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A60" s="2">
+        <v>0</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A61" s="2">
+        <v>0</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A62" s="2">
+        <v>1</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A63" s="2">
+        <v>1</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A64" s="2">
+        <v>1</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A65" s="5">
+        <v>1</v>
+      </c>
+      <c r="B65" s="5">
+        <v>1</v>
+      </c>
+      <c r="C65" s="5">
+        <v>1</v>
+      </c>
+      <c r="D65" s="5">
+        <v>1</v>
+      </c>
+      <c r="E65" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="7">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>